<commit_message>
chinh sua yeu cau in ra header_footer
</commit_message>
<xml_diff>
--- a/header_footer.xlsx
+++ b/header_footer.xlsx
@@ -21,13 +21,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>----------------header-----------------</t>
-  </si>
-  <si>
     <t>----------------end header-----------------</t>
-  </si>
-  <si>
-    <t>----------------footer-----------------</t>
   </si>
   <si>
     <t>----------------end footer-----------------</t>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>: 25-27-29 Tong Van Tran, Ward 5, District 11, HCMC</t>
+  </si>
+  <si>
+    <t>----------------begin header-----------------</t>
+  </si>
+  <si>
+    <t>----------------begin footer-----------------</t>
   </si>
 </sst>
 </file>
@@ -534,34 +534,34 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -573,42 +573,42 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>